<commit_message>
PRzygotowanie do poprawki  - do listy 5
</commit_message>
<xml_diff>
--- a/MRF17_L03.xlsx
+++ b/MRF17_L03.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Documents\Modelowanie rynków finansowych\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Documents\Modelowanie-rynkow-finansowych\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="1860" firstSheet="2" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="1860" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -376,9 +376,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -523,10 +523,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -1107,7 +1107,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1149,7 +1149,7 @@
         <v>56</v>
       </c>
       <c r="C1" s="19">
-        <v>8.9311203206651146E-2</v>
+        <v>8.9311203206651105E-2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1343,7 +1343,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B4:B15" si="1">1/(1+C5*(A5*7)/360)</f>
+        <f t="shared" ref="B5:B15" si="1">1/(1+C5*(A5*7)/360)</f>
         <v>0.99079931706057855</v>
       </c>
       <c r="C5">
@@ -1355,7 +1355,7 @@
         <v>4.2786391783946609E-2</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" ref="L5:L24" si="3">D5-$K$6</f>
+        <f t="shared" ref="L5:L15" si="3">D5-$K$6</f>
         <v>-7.2136082160533938E-3</v>
       </c>
       <c r="M5" s="21">
@@ -1824,7 +1824,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1864,7 +1864,7 @@
         <v>500</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E8" si="0">$A$2*C2*0.3</f>
+        <f>$A$2*C2*0.3</f>
         <v>1500</v>
       </c>
       <c r="F2">
@@ -1878,7 +1878,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3">
-        <f t="shared" ref="B3:B8" si="1">$A$2*C3*0.4</f>
+        <f t="shared" ref="B3:B8" si="0">$A$2*C3*0.4</f>
         <v>1920</v>
       </c>
       <c r="C3">
@@ -1889,7 +1889,7 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>$A$2*C3*0.3</f>
         <v>1440</v>
       </c>
       <c r="F3">
@@ -1903,18 +1903,18 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1960</v>
       </c>
       <c r="C4">
         <v>490</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D8" si="2">C3-C4</f>
+        <f t="shared" ref="D4:D8" si="1">C3-C4</f>
         <v>-10</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E2:E8" si="2">$A$2*C4*0.3</f>
         <v>1470</v>
       </c>
       <c r="F4">
@@ -1928,18 +1928,18 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2120</v>
       </c>
       <c r="C5">
         <v>530</v>
       </c>
       <c r="D5">
+        <f t="shared" si="1"/>
+        <v>-40</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="2"/>
-        <v>-40</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
         <v>1590</v>
       </c>
       <c r="F5">
@@ -1953,7 +1953,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2320</v>
       </c>
       <c r="C6">
@@ -1964,7 +1964,7 @@
         <v>-50</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1740</v>
       </c>
       <c r="F6">
@@ -1982,18 +1982,18 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2080</v>
       </c>
       <c r="C7">
         <v>520</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
         <v>1560</v>
       </c>
       <c r="F7">
@@ -2007,18 +2007,18 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1960</v>
       </c>
       <c r="C8">
         <v>490</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
         <v>1470</v>
       </c>
       <c r="F8">
@@ -2040,7 +2040,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2081,13 +2081,13 @@
       </c>
       <c r="B3">
         <f>B2+(E2-E3)*E1</f>
-        <v>2700.000000001135</v>
+        <v>2700.0000000012005</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
-        <v>26399.999999999622</v>
+        <v>26399.9999999996</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="E4">
         <f>E3/10</f>
-        <v>2639.9999999999623</v>
+        <v>2639.99999999996</v>
       </c>
     </row>
   </sheetData>
@@ -2109,7 +2109,7 @@
   <dimension ref="B1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2176,7 +2176,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2226,9 +2226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2250,7 +2248,7 @@
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>